<commit_message>
Large number of chages designed to get fiancial statements paid and align
</commit_message>
<xml_diff>
--- a/Santa_Clara_County_Charter_Schools.xlsx
+++ b/Santa_Clara_County_Charter_Schools.xlsx
@@ -8,8 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="School Data" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="School Data" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'School Data'!$A$1:$D$75</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="89">
   <si>
     <t xml:space="preserve">Authorizer</t>
   </si>
@@ -28,10 +31,10 @@
     <t xml:space="preserve">School Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Year Opened</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year Closed</t>
+    <t xml:space="preserve">Opened</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closed</t>
   </si>
   <si>
     <t xml:space="preserve">Cambrian</t>
@@ -121,7 +124,7 @@
     <t xml:space="preserve">KIPP Heartwood Academy</t>
   </si>
   <si>
-    <t xml:space="preserve">Santa Clara County Office of Education</t>
+    <t xml:space="preserve">SCCOE</t>
   </si>
   <si>
     <t xml:space="preserve">Bullis Charter</t>
@@ -262,15 +265,12 @@
     <t xml:space="preserve">Opportunity Youth Academy</t>
   </si>
   <si>
-    <t xml:space="preserve">SBE - Wei Yu International Charter</t>
+    <t xml:space="preserve">SBE</t>
   </si>
   <si>
     <t xml:space="preserve">Wei Yu International Charter</t>
   </si>
   <si>
-    <t xml:space="preserve">SBE - KIPP Navigate College Prep</t>
-  </si>
-  <si>
     <t xml:space="preserve">KIPP Navigate College Prep</t>
   </si>
   <si>
@@ -280,16 +280,16 @@
     <t xml:space="preserve">Legacy Academy</t>
   </si>
   <si>
-    <t xml:space="preserve">SBE - Promise Academy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Promise Academy</t>
   </si>
   <si>
-    <t xml:space="preserve">SBE - Perseverance Preparatory</t>
-  </si>
-  <si>
     <t xml:space="preserve">Perseverance Preparatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCCOE = Santa Clara County Office of Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBE = State Board of Education (California)</t>
   </si>
 </sst>
 </file>
@@ -301,7 +301,7 @@
     <numFmt numFmtId="165" formatCode="yyyy"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -360,7 +360,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="14"/>
+      <sz val="12"/>
       <name val="Alegreya Sans"/>
       <family val="2"/>
       <charset val="1"/>
@@ -368,6 +368,12 @@
     <font>
       <b val="true"/>
       <sz val="14"/>
+      <name val="Alegreya Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Alegreya Sans"/>
       <family val="2"/>
       <charset val="1"/>
@@ -460,73 +466,113 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -548,7 +594,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -556,7 +602,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -576,924 +622,1054 @@
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:XFD75"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="52.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="52.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="16.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="16.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="44.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="7.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="6.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="10.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="5" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+    <row r="1" s="9" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+    <row r="2" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="5" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="11"/>
-    </row>
-    <row r="7" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="11" t="n">
+      <c r="C14" s="12" t="n">
         <v>33848</v>
       </c>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="11" t="n">
+      <c r="C15" s="12" t="n">
         <v>35676</v>
       </c>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="11" t="n">
+      <c r="C16" s="12" t="n">
         <v>36768</v>
       </c>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="11" t="n">
+      <c r="C17" s="12" t="n">
         <v>37131</v>
       </c>
-      <c r="D17" s="11"/>
-    </row>
-    <row r="18" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9" t="s">
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="11" t="n">
+      <c r="C18" s="12" t="n">
         <v>37131</v>
       </c>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="11" t="n">
+      <c r="C19" s="12" t="n">
         <v>37438</v>
       </c>
-      <c r="D19" s="11"/>
-    </row>
-    <row r="20" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="11" t="n">
+      <c r="C20" s="12" t="n">
         <v>37495</v>
       </c>
-      <c r="D20" s="11"/>
-    </row>
-    <row r="21" s="12" customFormat="true" ht="35.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" s="13" customFormat="true" ht="28.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="11" t="n">
+      <c r="C21" s="12" t="n">
         <v>38223</v>
       </c>
-      <c r="D21" s="11"/>
-    </row>
-    <row r="22" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="11" t="n">
+      <c r="C22" s="12" t="n">
         <v>38224</v>
       </c>
-      <c r="D22" s="11"/>
-    </row>
-    <row r="23" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="10" t="s">
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="11" t="n">
+      <c r="C23" s="12" t="n">
         <v>38224</v>
       </c>
-      <c r="D23" s="11"/>
-    </row>
-    <row r="24" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="10" t="s">
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="11" t="n">
+      <c r="C24" s="12" t="n">
         <v>38224</v>
       </c>
-      <c r="D24" s="11" t="n">
+      <c r="D24" s="12" t="n">
         <v>42613</v>
       </c>
     </row>
-    <row r="25" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
+    <row r="25" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="11" t="n">
+      <c r="C25" s="12" t="n">
         <v>38237</v>
       </c>
-      <c r="D25" s="11"/>
-    </row>
-    <row r="26" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="10" t="s">
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="11" t="n">
+      <c r="C26" s="12" t="n">
         <v>38965</v>
       </c>
-      <c r="D26" s="11"/>
-    </row>
-    <row r="27" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="10" t="s">
+      <c r="D26" s="12"/>
+    </row>
+    <row r="27" s="17" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="11" t="n">
+      <c r="C27" s="16" t="n">
         <v>39295</v>
       </c>
-      <c r="D27" s="11"/>
-    </row>
-    <row r="28" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="10" t="s">
+      <c r="D27" s="16"/>
+    </row>
+    <row r="28" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="11" t="n">
+      <c r="C28" s="12" t="n">
         <v>39314</v>
       </c>
-      <c r="D28" s="11"/>
-    </row>
-    <row r="29" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="11" t="n">
+      <c r="C29" s="12" t="n">
         <v>39329</v>
       </c>
-      <c r="D29" s="11"/>
-    </row>
-    <row r="30" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
+      <c r="D29" s="12"/>
+    </row>
+    <row r="30" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="11" t="n">
+      <c r="C30" s="12" t="n">
         <v>39671</v>
       </c>
-      <c r="D30" s="11"/>
-    </row>
-    <row r="31" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="10" t="s">
+      <c r="D30" s="12"/>
+    </row>
+    <row r="31" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="11" t="n">
+      <c r="C31" s="12" t="n">
         <v>39686</v>
       </c>
-      <c r="D31" s="11"/>
-    </row>
-    <row r="32" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="10" t="s">
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" s="17" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="11" t="n">
+      <c r="C32" s="16" t="n">
         <v>40056</v>
       </c>
-      <c r="D32" s="11"/>
-    </row>
-    <row r="33" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="10" t="s">
+      <c r="D32" s="16"/>
+    </row>
+    <row r="33" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="11" t="n">
+      <c r="C33" s="12" t="n">
         <v>40406</v>
       </c>
-      <c r="D33" s="11" t="n">
+      <c r="D33" s="12" t="n">
         <v>42551</v>
       </c>
     </row>
-    <row r="34" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="10" t="s">
+    <row r="34" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="11" t="n">
+      <c r="C34" s="12" t="n">
         <v>40408</v>
       </c>
-      <c r="D34" s="11"/>
-    </row>
-    <row r="35" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="10" t="s">
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" s="17" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="11" t="n">
+      <c r="C35" s="16" t="n">
         <v>40415</v>
       </c>
-      <c r="D35" s="11"/>
-    </row>
-    <row r="36" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="s">
+      <c r="D35" s="16"/>
+    </row>
+    <row r="36" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="11" t="n">
+      <c r="C36" s="12" t="n">
         <v>40777</v>
       </c>
-      <c r="D36" s="11" t="n">
+      <c r="D36" s="12" t="n">
         <v>44012</v>
       </c>
     </row>
-    <row r="37" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="s">
+    <row r="37" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="11" t="n">
+      <c r="C37" s="12" t="n">
         <v>40777</v>
       </c>
-      <c r="D37" s="11"/>
-    </row>
-    <row r="38" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="10" t="s">
+      <c r="D37" s="12"/>
+    </row>
+    <row r="38" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="11" t="n">
+      <c r="C38" s="12" t="n">
         <v>40777</v>
       </c>
-      <c r="D38" s="11"/>
-    </row>
-    <row r="39" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="10" t="s">
+      <c r="D38" s="12"/>
+    </row>
+    <row r="39" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="11" t="n">
+      <c r="C39" s="12" t="n">
         <v>40777</v>
       </c>
-      <c r="D39" s="11"/>
-    </row>
-    <row r="40" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B40" s="10" t="s">
+      <c r="D39" s="12"/>
+    </row>
+    <row r="40" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="11" t="n">
+      <c r="C40" s="12" t="n">
         <v>40779</v>
       </c>
-      <c r="D40" s="11"/>
-    </row>
-    <row r="41" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="s">
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" s="17" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="11" t="n">
+      <c r="C41" s="16" t="n">
         <v>40784</v>
       </c>
-      <c r="D41" s="11"/>
-    </row>
-    <row r="42" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" s="10" t="s">
+      <c r="D41" s="16"/>
+    </row>
+    <row r="42" s="17" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="11" t="n">
+      <c r="C42" s="16" t="n">
         <v>40784</v>
       </c>
-      <c r="D42" s="11"/>
-    </row>
-    <row r="43" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" s="10" t="s">
+      <c r="D42" s="16"/>
+    </row>
+    <row r="43" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="11" t="n">
+      <c r="C43" s="12" t="n">
         <v>40792</v>
       </c>
-      <c r="D43" s="11" t="n">
+      <c r="D43" s="12" t="n">
         <v>42557</v>
       </c>
     </row>
-    <row r="44" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="10" t="s">
+    <row r="44" s="17" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="11" t="n">
+      <c r="C44" s="16" t="n">
         <v>41136</v>
       </c>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B45" s="10" t="s">
+      <c r="D44" s="16"/>
+    </row>
+    <row r="45" s="17" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="11" t="n">
+      <c r="C45" s="16" t="n">
         <v>41136</v>
       </c>
-      <c r="D45" s="11"/>
-    </row>
-    <row r="46" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="9" t="s">
+      <c r="D45" s="16"/>
+    </row>
+    <row r="46" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="11" t="n">
+      <c r="C46" s="12" t="n">
         <v>41141</v>
       </c>
-      <c r="D46" s="11"/>
-    </row>
-    <row r="47" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="9" t="s">
+      <c r="D46" s="12"/>
+    </row>
+    <row r="47" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="11" t="n">
+      <c r="C47" s="12" t="n">
         <v>41148</v>
       </c>
-      <c r="D47" s="11"/>
-    </row>
-    <row r="48" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9" t="s">
+      <c r="D47" s="12"/>
+    </row>
+    <row r="48" s="17" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="11" t="n">
+      <c r="C48" s="16" t="n">
         <v>41501</v>
       </c>
-      <c r="D48" s="11"/>
-    </row>
-    <row r="49" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B49" s="10" t="s">
+      <c r="D48" s="16"/>
+    </row>
+    <row r="49" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="11" t="n">
+      <c r="C49" s="12" t="n">
         <v>41505</v>
       </c>
-      <c r="D49" s="11" t="n">
+      <c r="D49" s="12" t="n">
         <v>45107</v>
       </c>
     </row>
-    <row r="50" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B50" s="10" t="s">
+    <row r="50" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="11" t="n">
+      <c r="C50" s="12" t="n">
         <v>41506</v>
       </c>
-      <c r="D50" s="11"/>
-    </row>
-    <row r="51" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9" t="s">
+      <c r="D50" s="12"/>
+    </row>
+    <row r="51" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="11" t="n">
+      <c r="C51" s="12" t="n">
         <v>41821</v>
       </c>
-      <c r="D51" s="11" t="n">
+      <c r="D51" s="12" t="n">
         <v>42551</v>
       </c>
     </row>
-    <row r="52" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9" t="s">
+    <row r="52" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C52" s="11" t="n">
+      <c r="C52" s="12" t="n">
         <v>41821</v>
       </c>
-      <c r="D52" s="11"/>
-    </row>
-    <row r="53" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B53" s="10" t="s">
+      <c r="D52" s="12"/>
+    </row>
+    <row r="53" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C53" s="11" t="n">
+      <c r="C53" s="12" t="n">
         <v>41848</v>
       </c>
-      <c r="D53" s="11"/>
-    </row>
-    <row r="54" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9" t="s">
+      <c r="D53" s="12"/>
+    </row>
+    <row r="54" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="11" t="n">
+      <c r="C54" s="12" t="n">
         <v>41852</v>
       </c>
-      <c r="D54" s="11"/>
-    </row>
-    <row r="55" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="s">
+      <c r="D54" s="12"/>
+    </row>
+    <row r="55" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C55" s="11" t="n">
+      <c r="C55" s="12" t="n">
         <v>41852</v>
       </c>
-      <c r="D55" s="11"/>
-    </row>
-    <row r="56" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="9" t="s">
+      <c r="D55" s="12"/>
+    </row>
+    <row r="56" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C56" s="11" t="n">
+      <c r="C56" s="12" t="n">
         <v>41862</v>
       </c>
-      <c r="D56" s="11"/>
-    </row>
-    <row r="57" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9" t="s">
+      <c r="D56" s="12"/>
+    </row>
+    <row r="57" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C57" s="11" t="n">
+      <c r="C57" s="12" t="n">
         <v>41869</v>
       </c>
-      <c r="D57" s="11"/>
-    </row>
-    <row r="58" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B58" s="10" t="s">
+      <c r="D57" s="12"/>
+    </row>
+    <row r="58" s="17" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B58" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C58" s="11" t="n">
+      <c r="C58" s="16" t="n">
         <v>41869</v>
       </c>
-      <c r="D58" s="11"/>
-    </row>
-    <row r="59" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
+      <c r="D58" s="16"/>
+    </row>
+    <row r="59" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C59" s="11" t="n">
+      <c r="C59" s="12" t="n">
         <v>42219</v>
       </c>
-      <c r="D59" s="11"/>
-    </row>
-    <row r="60" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9" t="s">
+      <c r="D59" s="12"/>
+    </row>
+    <row r="60" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C60" s="11" t="n">
+      <c r="C60" s="12" t="n">
         <v>42219</v>
       </c>
-      <c r="D60" s="11"/>
-    </row>
-    <row r="61" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="9" t="s">
+      <c r="D60" s="12"/>
+    </row>
+    <row r="61" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C61" s="11" t="n">
+      <c r="C61" s="12" t="n">
         <v>42219</v>
       </c>
-      <c r="D61" s="11"/>
-    </row>
-    <row r="62" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B62" s="10" t="s">
+      <c r="D61" s="12"/>
+    </row>
+    <row r="62" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C62" s="11" t="n">
+      <c r="C62" s="12" t="n">
         <v>42234</v>
       </c>
-      <c r="D62" s="11" t="n">
+      <c r="D62" s="12" t="n">
         <v>43281</v>
       </c>
     </row>
-    <row r="63" s="12" customFormat="true" ht="35.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B63" s="10" t="s">
+    <row r="63" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C63" s="11" t="n">
+      <c r="C63" s="12" t="n">
         <v>42255</v>
       </c>
-      <c r="D63" s="11"/>
-    </row>
-    <row r="64" s="12" customFormat="true" ht="35.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B64" s="10" t="s">
+      <c r="D63" s="12"/>
+    </row>
+    <row r="64" s="13" customFormat="true" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C64" s="11" t="n">
+      <c r="C64" s="12" t="n">
         <v>42255</v>
       </c>
-      <c r="D64" s="11"/>
-    </row>
-    <row r="65" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B65" s="10" t="s">
+      <c r="D64" s="12"/>
+    </row>
+    <row r="65" s="17" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C65" s="11" t="n">
+      <c r="C65" s="16" t="n">
         <v>42597</v>
       </c>
-      <c r="D65" s="11"/>
-    </row>
-    <row r="66" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B66" s="10" t="s">
+      <c r="D65" s="16"/>
+    </row>
+    <row r="66" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B66" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C66" s="11" t="n">
+      <c r="C66" s="12" t="n">
         <v>42614</v>
       </c>
-      <c r="D66" s="11"/>
-    </row>
-    <row r="67" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="9" t="s">
+      <c r="D66" s="12"/>
+    </row>
+    <row r="67" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C67" s="11" t="n">
+      <c r="C67" s="12" t="n">
         <v>42835</v>
       </c>
-      <c r="D67" s="11" t="n">
+      <c r="D67" s="12" t="n">
         <v>42835</v>
       </c>
     </row>
-    <row r="68" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="9" t="s">
+    <row r="68" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="C68" s="12" t="n">
+        <v>43326</v>
+      </c>
+      <c r="D68" s="12"/>
+    </row>
+    <row r="69" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C68" s="11" t="n">
-        <v>43326</v>
-      </c>
-      <c r="D68" s="11"/>
-    </row>
-    <row r="69" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B69" s="10" t="s">
+      <c r="C69" s="12" t="n">
+        <v>43332</v>
+      </c>
+      <c r="D69" s="12"/>
+    </row>
+    <row r="70" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B70" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C69" s="11" t="n">
-        <v>43332</v>
-      </c>
-      <c r="D69" s="11"/>
-    </row>
-    <row r="70" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B70" s="10" t="s">
+      <c r="C70" s="12" t="n">
+        <v>43341</v>
+      </c>
+      <c r="D70" s="12" t="n">
+        <v>43539</v>
+      </c>
+    </row>
+    <row r="71" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C70" s="11" t="n">
-        <v>43341</v>
-      </c>
-      <c r="D70" s="11" t="n">
-        <v>43539</v>
-      </c>
-    </row>
-    <row r="71" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="9" t="s">
+      <c r="C71" s="12" t="n">
+        <v>43678</v>
+      </c>
+      <c r="D71" s="12" t="n">
+        <v>43678</v>
+      </c>
+    </row>
+    <row r="72" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="C72" s="12" t="n">
+        <v>43691</v>
+      </c>
+      <c r="D72" s="12" t="n">
+        <v>45107</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="18"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="21"/>
+    </row>
+    <row r="74" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="C71" s="11" t="n">
-        <v>43678</v>
-      </c>
-      <c r="D71" s="11" t="n">
-        <v>43678</v>
-      </c>
-    </row>
-    <row r="72" s="12" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="9" t="s">
+      <c r="B74" s="22"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="25"/>
+      <c r="XFC74" s="25"/>
+      <c r="XFD74" s="25"/>
+    </row>
+    <row r="75" s="26" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B72" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C72" s="11" t="n">
-        <v>43691</v>
-      </c>
-      <c r="D72" s="11" t="n">
-        <v>45107</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="13"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="16"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="25"/>
+      <c r="XFC75" s="25"/>
+      <c r="XFD75" s="25"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>